<commit_message>
updates to correct defaulting to 0
</commit_message>
<xml_diff>
--- a/posting_script/event_schedule.xlsx
+++ b/posting_script/event_schedule.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slipstreaminc2-my.sharepoint.com/personal/bbartling_slipstreaminc_org/Documents/Desktop/bacnet-demand-response-client/posting_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A2EAD81-E89C-40BE-95AB-6DA60F755787}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{827D3191-8749-46C5-A3C2-611AE3DDE80E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="slipstream_event_schedule" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">slipstream_event_schedule!$A$1:$A$97</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -869,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -888,7 +891,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -896,7 +899,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45154.010416666664</v>
+        <v>45155.010416666664</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -904,7 +907,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45154.020833333336</v>
+        <v>45155.020833333336</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -912,7 +915,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45154.03125</v>
+        <v>45155.03125</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -920,7 +923,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45154.041666666664</v>
+        <v>45155.041666666664</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -928,7 +931,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45154.052083333336</v>
+        <v>45155.052083333336</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -936,7 +939,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45154.0625</v>
+        <v>45155.0625</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -944,7 +947,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45154.072916666664</v>
+        <v>45155.072916666664</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -952,7 +955,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45154.083333333336</v>
+        <v>45155.083333333336</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -960,7 +963,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45154.09375</v>
+        <v>45155.09375</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -968,7 +971,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45154.104166666664</v>
+        <v>45155.104166666664</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -976,7 +979,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45154.114583333336</v>
+        <v>45155.114583333336</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -984,7 +987,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45154.125</v>
+        <v>45155.125</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -992,7 +995,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45154.135416666664</v>
+        <v>45155.135416666664</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1000,7 +1003,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45154.145833333336</v>
+        <v>45155.145833333336</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1008,7 +1011,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45154.15625</v>
+        <v>45155.15625</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1016,7 +1019,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>45154.166666666664</v>
+        <v>45155.166666666664</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1024,7 +1027,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>45154.177083333336</v>
+        <v>45155.177083333336</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1032,7 +1035,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>45154.1875</v>
+        <v>45155.1875</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1040,7 +1043,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>45154.197916666664</v>
+        <v>45155.197916666664</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1048,7 +1051,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>45154.208333333336</v>
+        <v>45155.208333333336</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1056,7 +1059,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>45154.21875</v>
+        <v>45155.21875</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>45154.229166666664</v>
+        <v>45155.229166666664</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1072,7 +1075,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>45154.239583333336</v>
+        <v>45155.239583333336</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1080,7 +1083,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>45154.25</v>
+        <v>45155.25</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1088,7 +1091,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>45154.260416666664</v>
+        <v>45155.260416666664</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1096,7 +1099,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>45154.270833333336</v>
+        <v>45155.270833333336</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1104,7 +1107,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>45154.28125</v>
+        <v>45155.28125</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>45154.291666666664</v>
+        <v>45155.291666666664</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1120,7 +1123,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>45154.302083333336</v>
+        <v>45155.302083333336</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1128,7 +1131,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>45154.3125</v>
+        <v>45155.3125</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1136,7 +1139,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>45154.322916666664</v>
+        <v>45155.322916666664</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1144,7 +1147,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>45154.333333333336</v>
+        <v>45155.333333333336</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1152,7 +1155,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>45154.34375</v>
+        <v>45155.34375</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>45154.354166666664</v>
+        <v>45155.354166666664</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1168,7 +1171,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>45154.364583333336</v>
+        <v>45155.364583333336</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1176,7 +1179,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>45154.375</v>
+        <v>45155.375</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1184,7 +1187,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>45154.385416666664</v>
+        <v>45155.385416666664</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>45154.395833333336</v>
+        <v>45155.395833333336</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1200,7 +1203,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>45154.40625</v>
+        <v>45155.40625</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1208,7 +1211,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>45154.416666666664</v>
+        <v>45155.416666666664</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1216,7 +1219,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>45154.427083333336</v>
+        <v>45155.427083333336</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1224,7 +1227,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>45154.4375</v>
+        <v>45155.4375</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1232,7 +1235,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>45154.447916666664</v>
+        <v>45155.447916666664</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1240,7 +1243,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>45154.458333333336</v>
+        <v>45155.458333333336</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1248,7 +1251,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>45154.46875</v>
+        <v>45155.46875</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1256,7 +1259,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>45154.479166666664</v>
+        <v>45155.479166666664</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1264,7 +1267,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>45154.489583333336</v>
+        <v>45155.489583333336</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1272,7 +1275,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>45154.5</v>
+        <v>45155.5</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1280,7 +1283,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>45154.510416666664</v>
+        <v>45155.510416666664</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1288,7 +1291,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>45154.520833333336</v>
+        <v>45155.520833333336</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1296,7 +1299,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>45154.53125</v>
+        <v>45155.53125</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1304,71 +1307,71 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>45154.541666666664</v>
+        <v>45155.541666666664</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>45154.552083333336</v>
+        <v>45155.552083333336</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>45154.5625</v>
+        <v>45155.5625</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>45154.572916666664</v>
+        <v>45155.572916666664</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>45154.583333333336</v>
+        <v>45155.583333333336</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>45154.59375</v>
+        <v>45155.59375</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>45154.604166666664</v>
+        <v>45155.604166666664</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>45154.614583333336</v>
+        <v>45155.614583333336</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>45154.625</v>
+        <v>45155.625</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1376,7 +1379,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>45154.635416666664</v>
+        <v>45155.635416666664</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1384,7 +1387,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>45154.645833333336</v>
+        <v>45155.645833333336</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1392,7 +1395,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>45154.65625</v>
+        <v>45155.65625</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1400,103 +1403,103 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>45154.666666666664</v>
+        <v>45155.666666666664</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>45154.677083333336</v>
+        <v>45155.677083333336</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>45154.6875</v>
+        <v>45155.6875</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>45154.697916666664</v>
+        <v>45155.697916666664</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>45154.708333333336</v>
+        <v>45155.708333333336</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>45154.71875</v>
+        <v>45155.71875</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>45154.729166666664</v>
+        <v>45155.729166666664</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>45154.739583333336</v>
+        <v>45155.739583333336</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>45154.75</v>
+        <v>45155.75</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>45154.760416666664</v>
+        <v>45155.760416666664</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>45154.770833333336</v>
+        <v>45155.770833333336</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>45154.78125</v>
+        <v>45155.78125</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>45154.791666666664</v>
+        <v>45155.791666666664</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1504,7 +1507,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>45154.802083333336</v>
+        <v>45155.802083333336</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1512,7 +1515,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>45154.8125</v>
+        <v>45155.8125</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1520,7 +1523,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>45154.822916666664</v>
+        <v>45155.822916666664</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1528,71 +1531,71 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>45154.833333333336</v>
+        <v>45155.833333333336</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>45154.84375</v>
+        <v>45155.84375</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>45154.854166666664</v>
+        <v>45155.854166666664</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>45154.864583333336</v>
+        <v>45155.864583333336</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>45154.875</v>
+        <v>45155.875</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>45154.885416666664</v>
+        <v>45155.885416666664</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>45154.895833333336</v>
+        <v>45155.895833333336</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>45154.90625</v>
+        <v>45155.90625</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>45154.916666666664</v>
+        <v>45155.916666666664</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1600,7 +1603,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>45154.927083333336</v>
+        <v>45155.927083333336</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1608,7 +1611,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>45154.9375</v>
+        <v>45155.9375</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1616,7 +1619,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>45154.947916666664</v>
+        <v>45155.947916666664</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>45154.958333333336</v>
+        <v>45155.958333333336</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1632,7 +1635,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>45154.96875</v>
+        <v>45155.96875</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1640,7 +1643,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>45154.979166666664</v>
+        <v>45155.979166666664</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1648,7 +1651,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>45154.989583333336</v>
+        <v>45155.989583333336</v>
       </c>
       <c r="B97">
         <v>0</v>

</xml_diff>

<commit_message>
updated bacnet server readme
</commit_message>
<xml_diff>
--- a/posting_script/event_schedule.xlsx
+++ b/posting_script/event_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slipstreaminc2-my.sharepoint.com/personal/bbartling_slipstreaminc_org/Documents/Desktop/bacnet-demand-response-client/posting_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{827D3191-8749-46C5-A3C2-611AE3DDE80E}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BFA1F0C-0776-4B13-B978-174CBA1A3F35}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,7 +891,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45155</v>
+        <v>45156</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45155.010416666664</v>
+        <v>45156.010416666664</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45155.020833333336</v>
+        <v>45156.020833333336</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45155.03125</v>
+        <v>45156.03125</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45155.041666666664</v>
+        <v>45156.041666666664</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>45155.052083333336</v>
+        <v>45156.052083333336</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>45155.0625</v>
+        <v>45156.0625</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>45155.072916666664</v>
+        <v>45156.072916666664</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>45155.083333333336</v>
+        <v>45156.083333333336</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45155.09375</v>
+        <v>45156.09375</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>45155.104166666664</v>
+        <v>45156.104166666664</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>45155.114583333336</v>
+        <v>45156.114583333336</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45155.125</v>
+        <v>45156.125</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>45155.135416666664</v>
+        <v>45156.135416666664</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>45155.145833333336</v>
+        <v>45156.145833333336</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>45155.15625</v>
+        <v>45156.15625</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>45155.166666666664</v>
+        <v>45156.166666666664</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>45155.177083333336</v>
+        <v>45156.177083333336</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>45155.1875</v>
+        <v>45156.1875</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>45155.197916666664</v>
+        <v>45156.197916666664</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>45155.208333333336</v>
+        <v>45156.208333333336</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>45155.21875</v>
+        <v>45156.21875</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>45155.229166666664</v>
+        <v>45156.229166666664</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>45155.239583333336</v>
+        <v>45156.239583333336</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>45155.25</v>
+        <v>45156.25</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>45155.260416666664</v>
+        <v>45156.260416666664</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>45155.270833333336</v>
+        <v>45156.270833333336</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>45155.28125</v>
+        <v>45156.28125</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>45155.291666666664</v>
+        <v>45156.291666666664</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>45155.302083333336</v>
+        <v>45156.302083333336</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>45155.3125</v>
+        <v>45156.3125</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>45155.322916666664</v>
+        <v>45156.322916666664</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>45155.333333333336</v>
+        <v>45156.333333333336</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>45155.34375</v>
+        <v>45156.34375</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>45155.354166666664</v>
+        <v>45156.354166666664</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>45155.364583333336</v>
+        <v>45156.364583333336</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>45155.375</v>
+        <v>45156.375</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>45155.385416666664</v>
+        <v>45156.385416666664</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>45155.395833333336</v>
+        <v>45156.395833333336</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>45155.40625</v>
+        <v>45156.40625</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>45155.416666666664</v>
+        <v>45156.416666666664</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>45155.427083333336</v>
+        <v>45156.427083333336</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>45155.4375</v>
+        <v>45156.4375</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>45155.447916666664</v>
+        <v>45156.447916666664</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>45155.458333333336</v>
+        <v>45156.458333333336</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>45155.46875</v>
+        <v>45156.46875</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>45155.479166666664</v>
+        <v>45156.479166666664</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>45155.489583333336</v>
+        <v>45156.489583333336</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>45155.5</v>
+        <v>45156.5</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>45155.510416666664</v>
+        <v>45156.510416666664</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>45155.520833333336</v>
+        <v>45156.520833333336</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>45155.53125</v>
+        <v>45156.53125</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>45155.541666666664</v>
+        <v>45156.541666666664</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>45155.552083333336</v>
+        <v>45156.552083333336</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>45155.5625</v>
+        <v>45156.5625</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>45155.572916666664</v>
+        <v>45156.572916666664</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>45155.583333333336</v>
+        <v>45156.583333333336</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>45155.59375</v>
+        <v>45156.59375</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>45155.604166666664</v>
+        <v>45156.604166666664</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>45155.614583333336</v>
+        <v>45156.614583333336</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>45155.625</v>
+        <v>45156.625</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>45155.635416666664</v>
+        <v>45156.635416666664</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>45155.645833333336</v>
+        <v>45156.645833333336</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>45155.65625</v>
+        <v>45156.65625</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>45155.666666666664</v>
+        <v>45156.666666666664</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>45155.677083333336</v>
+        <v>45156.677083333336</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>45155.6875</v>
+        <v>45156.6875</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>45155.697916666664</v>
+        <v>45156.697916666664</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>45155.708333333336</v>
+        <v>45156.708333333336</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>45155.71875</v>
+        <v>45156.71875</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>45155.729166666664</v>
+        <v>45156.729166666664</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>45155.739583333336</v>
+        <v>45156.739583333336</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>45155.75</v>
+        <v>45156.75</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>45155.760416666664</v>
+        <v>45156.760416666664</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>45155.770833333336</v>
+        <v>45156.770833333336</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>45155.78125</v>
+        <v>45156.78125</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>45155.791666666664</v>
+        <v>45156.791666666664</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>45155.802083333336</v>
+        <v>45156.802083333336</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>45155.8125</v>
+        <v>45156.8125</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>45155.822916666664</v>
+        <v>45156.822916666664</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>45155.833333333336</v>
+        <v>45156.833333333336</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>45155.84375</v>
+        <v>45156.84375</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>45155.854166666664</v>
+        <v>45156.854166666664</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>45155.864583333336</v>
+        <v>45156.864583333336</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>45155.875</v>
+        <v>45156.875</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>45155.885416666664</v>
+        <v>45156.885416666664</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>45155.895833333336</v>
+        <v>45156.895833333336</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>45155.90625</v>
+        <v>45156.90625</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>45155.916666666664</v>
+        <v>45156.916666666664</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>45155.927083333336</v>
+        <v>45156.927083333336</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>45155.9375</v>
+        <v>45156.9375</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>45155.947916666664</v>
+        <v>45156.947916666664</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>45155.958333333336</v>
+        <v>45156.958333333336</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>45155.96875</v>
+        <v>45156.96875</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>45155.979166666664</v>
+        <v>45156.979166666664</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>45155.989583333336</v>
+        <v>45156.989583333336</v>
       </c>
       <c r="B97">
         <v>0</v>

</xml_diff>

<commit_message>
app should be ready for field testing
</commit_message>
<xml_diff>
--- a/posting_script/event_schedule.xlsx
+++ b/posting_script/event_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slipstreaminc2-my.sharepoint.com/personal/bbartling_slipstreaminc_org/Documents/Desktop/bacnet-demand-response-client/posting_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BFA1F0C-0776-4B13-B978-174CBA1A3F35}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52650D9-E78A-4ACA-9649-EFE911FDF213}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -873,7 +873,7 @@
   <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,7 +998,7 @@
         <v>45156.135416666664</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1006,7 +1006,7 @@
         <v>45156.145833333336</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1014,7 +1014,7 @@
         <v>45156.15625</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1022,7 +1022,7 @@
         <v>45156.166666666664</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1030,7 +1030,7 @@
         <v>45156.177083333336</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1038,7 +1038,7 @@
         <v>45156.1875</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
         <v>45156.197916666664</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1054,7 +1054,7 @@
         <v>45156.208333333336</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1062,7 +1062,7 @@
         <v>45156.21875</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1070,7 +1070,7 @@
         <v>45156.229166666664</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1078,7 +1078,7 @@
         <v>45156.239583333336</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>45156.25</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1094,7 +1094,7 @@
         <v>45156.260416666664</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>